<commit_message>
Update to sample data
</commit_message>
<xml_diff>
--- a/b_Data_Sample/Sample_Dataset_TextBased_AdFeedback_TopicModeling.xlsx
+++ b/b_Data_Sample/Sample_Dataset_TextBased_AdFeedback_TopicModeling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RescueRebece_SD/Desktop/DS_Course/TextBased_AdFeedback_TopicModeling/b. Data_Sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RescueRebece_SD/Desktop/DS_Course/TextBased_AdFeedback_TopicModeling/b_Data_Sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AFEB54-5BAD-9045-812E-A572849EC506}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39F1F3B-C307-2343-B944-6DD4503D2BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="25600" windowHeight="14680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -77,24 +77,12 @@
     <t>Question</t>
   </si>
   <si>
-    <t>I like the actors</t>
-  </si>
-  <si>
     <t>DD</t>
   </si>
   <si>
-    <t>Likes</t>
-  </si>
-  <si>
-    <t>Too long</t>
-  </si>
-  <si>
     <t>DF</t>
   </si>
   <si>
-    <t>Dislikes</t>
-  </si>
-  <si>
     <t>It's not safe to vape</t>
   </si>
   <si>
@@ -104,7 +92,13 @@
     <t>Main Message</t>
   </si>
   <si>
-    <t>It was straight-forward</t>
+    <t>vaping can be dangerous to immune system</t>
+  </si>
+  <si>
+    <t>dishonesty in industry</t>
+  </si>
+  <si>
+    <t>the harms of vaping to your lungs</t>
   </si>
 </sst>
 </file>
@@ -122,16 +116,19 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -389,7 +386,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -524,7 +521,9 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -551,13 +550,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -565,13 +564,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -579,13 +578,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -593,13 +592,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>